<commit_message>
added data, changed metadata, change file structures in photogrammetry/data folder
</commit_message>
<xml_diff>
--- a/settlementTiles/data/settlementTileMetadata.xlsx
+++ b/settlementTiles/data/settlementTileMetadata.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iancombs/Documents/GitHub/photogrammetryNOAA/settlementTiles/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0097390D-5821-8943-A3B6-0BB849B1AC0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{14002841-A8AC-FA4C-B9A3-AC9A7B7097F1}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="27645" windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -60,12 +54,33 @@
   </si>
   <si>
     <t>IC-Z2</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>100-112</t>
+  </si>
+  <si>
+    <t>200-212</t>
+  </si>
+  <si>
+    <t>300-312</t>
+  </si>
+  <si>
+    <t>400-412</t>
+  </si>
+  <si>
+    <t>500-512</t>
+  </si>
+  <si>
+    <t>600-612</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -405,23 +420,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E073B8-13F3-7945-A8E9-F2A58D014429}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +446,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44047</v>
       </c>
@@ -442,8 +460,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44047</v>
       </c>
@@ -453,8 +474,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44047</v>
       </c>
@@ -464,8 +488,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44047</v>
       </c>
@@ -475,8 +502,11 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44047</v>
       </c>
@@ -486,8 +516,11 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44047</v>
       </c>
@@ -496,6 +529,9 @@
       </c>
       <c r="C7" t="s">
         <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated settlement tile metadata
</commit_message>
<xml_diff>
--- a/settlementTiles/data/settlementTileMetadata.xlsx
+++ b/settlementTiles/data/settlementTileMetadata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>date</t>
   </si>
@@ -59,22 +59,94 @@
     <t>Series</t>
   </si>
   <si>
-    <t>100-112</t>
-  </si>
-  <si>
-    <t>200-212</t>
-  </si>
-  <si>
-    <t>300-312</t>
-  </si>
-  <si>
-    <t>400-412</t>
-  </si>
-  <si>
-    <t>500-512</t>
-  </si>
-  <si>
-    <t>600-612</t>
+    <t>IC-Z3</t>
+  </si>
+  <si>
+    <t>IC-C3</t>
+  </si>
+  <si>
+    <t>IC-U3</t>
+  </si>
+  <si>
+    <t>101-112-1</t>
+  </si>
+  <si>
+    <t>201-212-1</t>
+  </si>
+  <si>
+    <t>301-312-1</t>
+  </si>
+  <si>
+    <t>401-412-1</t>
+  </si>
+  <si>
+    <t>501-512-1</t>
+  </si>
+  <si>
+    <t>601-612-1</t>
+  </si>
+  <si>
+    <t>501-512-2</t>
+  </si>
+  <si>
+    <t>601-612-2</t>
+  </si>
+  <si>
+    <t>301-312-2</t>
+  </si>
+  <si>
+    <t>401-412-2</t>
+  </si>
+  <si>
+    <t>101-112-2</t>
+  </si>
+  <si>
+    <t>201-212-2</t>
+  </si>
+  <si>
+    <t>101-112-3</t>
+  </si>
+  <si>
+    <t>201-212-3</t>
+  </si>
+  <si>
+    <t>301-312-3</t>
+  </si>
+  <si>
+    <t>401-412-3</t>
+  </si>
+  <si>
+    <t>501-512-3</t>
+  </si>
+  <si>
+    <t>601-612-3</t>
+  </si>
+  <si>
+    <t>601-612-4</t>
+  </si>
+  <si>
+    <t>501-512-4</t>
+  </si>
+  <si>
+    <t>901-912-1</t>
+  </si>
+  <si>
+    <t>401-412-4</t>
+  </si>
+  <si>
+    <t>801-812-1</t>
+  </si>
+  <si>
+    <t>301-312-4</t>
+  </si>
+  <si>
+    <t>201-212-4</t>
+  </si>
+  <si>
+    <t>701-712-1</t>
+  </si>
+  <si>
+    <t>101-112-4</t>
   </si>
 </sst>
 </file>
@@ -420,7 +492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -461,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -475,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -489,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -503,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,7 +603,274 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44208</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44208</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44208</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44319</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>